<commit_message>
new readings has arrived
</commit_message>
<xml_diff>
--- a/new test/Azotu tekrarlananlar.xlsx
+++ b/new test/Azotu tekrarlananlar.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ugurg\Documents\GitHub\oceanview\new test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{924DF638-F6B7-4702-A076-1F2D8DF9BFD3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98A92E5-6631-4DB4-8474-655BE1FDDE2D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2550" yWindow="2550" windowWidth="13440" windowHeight="11385" xr2:uid="{A05D719E-45E3-4720-854B-F71AD97E7A96}"/>
+    <workbookView xWindow="-6465" yWindow="4035" windowWidth="13440" windowHeight="11385" xr2:uid="{A05D719E-45E3-4720-854B-F71AD97E7A96}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="72">
   <si>
     <t>Lab no</t>
   </si>
@@ -351,7 +351,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
@@ -396,6 +396,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -710,11 +724,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{289753B6-3BB7-49B3-920D-C731DAECE199}">
-  <dimension ref="A1:U76"/>
+  <dimension ref="A1:U77"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J47" sqref="J47"/>
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -919,93 +933,69 @@
         <v>74.959999999999994</v>
       </c>
     </row>
-    <row r="5" spans="1:21">
-      <c r="A5" s="4">
-        <v>2391</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="D5" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.34</v>
-      </c>
-      <c r="F5" s="6">
-        <v>7.54</v>
-      </c>
-      <c r="G5" s="7">
-        <v>3.9699999999999999E-2</v>
-      </c>
-      <c r="H5" s="8">
-        <v>1.17</v>
-      </c>
-      <c r="I5" s="6">
-        <v>7.07</v>
-      </c>
-      <c r="J5" s="8">
-        <v>46.328000000000003</v>
-      </c>
-      <c r="K5" s="8">
-        <v>31.744</v>
-      </c>
-      <c r="L5" s="8">
-        <v>21.928000000000001</v>
-      </c>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-      <c r="Q5" s="4"/>
-      <c r="R5" s="4"/>
-      <c r="S5" s="4"/>
-      <c r="T5" s="6">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="U5" s="6">
-        <v>77.28</v>
-      </c>
+    <row r="5" spans="1:21" s="15" customFormat="1">
+      <c r="A5" s="14">
+        <v>2390</v>
+      </c>
+      <c r="B5" s="14"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="14"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="21"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="20"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="14"/>
+      <c r="N5" s="14"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="4">
-        <v>2392</v>
+        <v>2391</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D6" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E6" s="4">
-        <v>0.5</v>
+        <v>0.34</v>
       </c>
       <c r="F6" s="6">
-        <v>7.73</v>
+        <v>7.54</v>
       </c>
       <c r="G6" s="7">
-        <v>3.6600000000000001E-2</v>
+        <v>3.9699999999999999E-2</v>
       </c>
       <c r="H6" s="8">
-        <v>0.97</v>
+        <v>1.17</v>
       </c>
       <c r="I6" s="6">
-        <v>9.75</v>
+        <v>7.07</v>
       </c>
       <c r="J6" s="8">
-        <v>32.328000000000003</v>
+        <v>46.328000000000003</v>
       </c>
       <c r="K6" s="8">
-        <v>35.744</v>
+        <v>31.744</v>
       </c>
       <c r="L6" s="8">
-        <v>31.928000000000001</v>
+        <v>21.928000000000001</v>
       </c>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
@@ -1015,48 +1005,48 @@
       <c r="R6" s="4"/>
       <c r="S6" s="4"/>
       <c r="T6" s="6">
-        <v>9.5</v>
+        <v>18.420000000000002</v>
       </c>
       <c r="U6" s="6">
-        <v>59.92</v>
+        <v>77.28</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="4">
-        <v>2393</v>
+        <v>2392</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D7" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E7" s="4">
-        <v>0.39</v>
+        <v>0.5</v>
       </c>
       <c r="F7" s="6">
-        <v>7.45</v>
+        <v>7.73</v>
       </c>
       <c r="G7" s="7">
-        <v>4.3299999999999998E-2</v>
+        <v>3.6600000000000001E-2</v>
       </c>
       <c r="H7" s="8">
-        <v>1.29</v>
+        <v>0.97</v>
       </c>
       <c r="I7" s="6">
-        <v>6.5</v>
+        <v>9.75</v>
       </c>
       <c r="J7" s="8">
-        <v>64.328000000000003</v>
+        <v>32.328000000000003</v>
       </c>
       <c r="K7" s="8">
-        <v>11.744</v>
+        <v>35.744</v>
       </c>
       <c r="L7" s="8">
-        <v>23.928000000000001</v>
+        <v>31.928000000000001</v>
       </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1066,48 +1056,48 @@
       <c r="R7" s="4"/>
       <c r="S7" s="4"/>
       <c r="T7" s="6">
-        <v>7.58</v>
+        <v>9.5</v>
       </c>
       <c r="U7" s="6">
-        <v>18.2</v>
+        <v>59.92</v>
       </c>
     </row>
     <row r="8" spans="1:21">
       <c r="A8" s="4">
-        <v>2394</v>
+        <v>2393</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E8" s="4">
-        <v>0.17</v>
+        <v>0.39</v>
       </c>
       <c r="F8" s="6">
-        <v>7.77</v>
+        <v>7.45</v>
       </c>
       <c r="G8" s="7">
-        <v>1.09E-2</v>
+        <v>4.3299999999999998E-2</v>
       </c>
       <c r="H8" s="8">
-        <v>0.31</v>
+        <v>1.29</v>
       </c>
       <c r="I8" s="6">
-        <v>7.0000000000000007E-2</v>
+        <v>6.5</v>
       </c>
       <c r="J8" s="8">
-        <v>32.328000000000003</v>
+        <v>64.328000000000003</v>
       </c>
       <c r="K8" s="8">
-        <v>25.744</v>
+        <v>11.744</v>
       </c>
       <c r="L8" s="8">
-        <v>41.927999999999997</v>
+        <v>23.928000000000001</v>
       </c>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
@@ -1117,48 +1107,48 @@
       <c r="R8" s="4"/>
       <c r="S8" s="4"/>
       <c r="T8" s="6">
-        <v>9.42</v>
+        <v>7.58</v>
       </c>
       <c r="U8" s="6">
-        <v>28.82</v>
+        <v>18.2</v>
       </c>
     </row>
     <row r="9" spans="1:21">
       <c r="A9" s="4">
-        <v>2395</v>
+        <v>2394</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="D9" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E9" s="4">
-        <v>0.39</v>
+        <v>0.17</v>
       </c>
       <c r="F9" s="6">
-        <v>7.65</v>
+        <v>7.77</v>
       </c>
       <c r="G9" s="7">
-        <v>2.8400000000000002E-2</v>
+        <v>1.09E-2</v>
       </c>
       <c r="H9" s="8">
-        <v>0.76</v>
+        <v>0.31</v>
       </c>
       <c r="I9" s="6">
-        <v>0.28000000000000003</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="J9" s="8">
-        <v>64.688000000000002</v>
+        <v>32.328000000000003</v>
       </c>
       <c r="K9" s="8">
-        <v>25.456</v>
+        <v>25.744</v>
       </c>
       <c r="L9" s="8">
-        <v>9.8559999999999999</v>
+        <v>41.927999999999997</v>
       </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1168,48 +1158,48 @@
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
       <c r="T9" s="6">
-        <v>10.67</v>
+        <v>9.42</v>
       </c>
       <c r="U9" s="6">
-        <v>47.75</v>
+        <v>28.82</v>
       </c>
     </row>
     <row r="10" spans="1:21">
       <c r="A10" s="4">
-        <v>2396</v>
+        <v>2395</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>29</v>
+        <v>47</v>
       </c>
       <c r="D10" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E10" s="4">
-        <v>0.56000000000000005</v>
+        <v>0.39</v>
       </c>
       <c r="F10" s="6">
-        <v>7.71</v>
+        <v>7.65</v>
       </c>
       <c r="G10" s="7">
-        <v>1.9199999999999998E-2</v>
+        <v>2.8400000000000002E-2</v>
       </c>
       <c r="H10" s="8">
-        <v>0.4</v>
+        <v>0.76</v>
       </c>
       <c r="I10" s="6">
-        <v>2.83</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="J10" s="8">
-        <v>24.687999999999999</v>
+        <v>64.688000000000002</v>
       </c>
       <c r="K10" s="8">
-        <v>47.456000000000003</v>
+        <v>25.456</v>
       </c>
       <c r="L10" s="8">
-        <v>27.856000000000002</v>
+        <v>9.8559999999999999</v>
       </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
@@ -1219,48 +1209,48 @@
       <c r="R10" s="4"/>
       <c r="S10" s="4"/>
       <c r="T10" s="6">
-        <v>10.83</v>
+        <v>10.67</v>
       </c>
       <c r="U10" s="6">
-        <v>49.17</v>
+        <v>47.75</v>
       </c>
     </row>
     <row r="11" spans="1:21">
       <c r="A11" s="4">
-        <v>2397</v>
+        <v>2396</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="D11" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E11" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F11" s="6">
-        <v>7.75</v>
+        <v>7.71</v>
       </c>
       <c r="G11" s="7">
-        <v>2.6700000000000002E-2</v>
+        <v>1.9199999999999998E-2</v>
       </c>
       <c r="H11" s="8">
-        <v>0.57999999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="I11" s="6">
-        <v>0.42</v>
+        <v>2.83</v>
       </c>
       <c r="J11" s="8">
-        <v>28.687999999999999</v>
+        <v>24.687999999999999</v>
       </c>
       <c r="K11" s="8">
-        <v>41.456000000000003</v>
+        <v>47.456000000000003</v>
       </c>
       <c r="L11" s="8">
-        <v>29.856000000000002</v>
+        <v>27.856000000000002</v>
       </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
@@ -1270,48 +1260,48 @@
       <c r="R11" s="4"/>
       <c r="S11" s="4"/>
       <c r="T11" s="6">
-        <v>14.25</v>
+        <v>10.83</v>
       </c>
       <c r="U11" s="6">
-        <v>54.11</v>
+        <v>49.17</v>
       </c>
     </row>
     <row r="12" spans="1:21">
       <c r="A12" s="4">
-        <v>2405</v>
+        <v>2397</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="D12" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E12" s="4">
-        <v>0.39</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F12" s="6">
-        <v>7.03</v>
+        <v>7.75</v>
       </c>
       <c r="G12" s="7">
-        <v>3.3300000000000003E-2</v>
+        <v>2.6700000000000002E-2</v>
       </c>
       <c r="H12" s="8">
-        <v>0.96</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I12" s="6">
         <v>0.42</v>
       </c>
       <c r="J12" s="8">
-        <v>26.687999999999999</v>
+        <v>28.687999999999999</v>
       </c>
       <c r="K12" s="8">
-        <v>33.456000000000003</v>
+        <v>41.456000000000003</v>
       </c>
       <c r="L12" s="8">
-        <v>39.856000000000002</v>
+        <v>29.856000000000002</v>
       </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
@@ -1321,45 +1311,45 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="6">
-        <v>12.75</v>
-      </c>
-      <c r="U12" s="9">
-        <v>28.09</v>
+        <v>14.25</v>
+      </c>
+      <c r="U12" s="6">
+        <v>54.11</v>
       </c>
     </row>
     <row r="13" spans="1:21">
       <c r="A13" s="4">
-        <v>2406</v>
+        <v>2405</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D13" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E13" s="4">
-        <v>0.22</v>
+        <v>0.39</v>
       </c>
       <c r="F13" s="6">
-        <v>6.61</v>
+        <v>7.03</v>
       </c>
       <c r="G13" s="7">
-        <v>2.2499999999999999E-2</v>
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="H13" s="8">
-        <v>0.63</v>
+        <v>0.96</v>
       </c>
       <c r="I13" s="6">
-        <v>0.14000000000000001</v>
+        <v>0.42</v>
       </c>
       <c r="J13" s="8">
-        <v>28.687999999999999</v>
+        <v>26.687999999999999</v>
       </c>
       <c r="K13" s="8">
-        <v>31.456</v>
+        <v>33.456000000000003</v>
       </c>
       <c r="L13" s="8">
         <v>39.856000000000002</v>
@@ -1372,48 +1362,48 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="6">
-        <v>22.58</v>
+        <v>12.75</v>
       </c>
       <c r="U13" s="9">
-        <v>19.46</v>
+        <v>28.09</v>
       </c>
     </row>
     <row r="14" spans="1:21">
       <c r="A14" s="4">
-        <v>2407</v>
+        <v>2406</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="D14" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E14" s="4">
-        <v>0.17</v>
+        <v>0.22</v>
       </c>
       <c r="F14" s="6">
-        <v>7.2</v>
+        <v>6.61</v>
       </c>
       <c r="G14" s="7">
-        <v>6.6299999999999998E-2</v>
+        <v>2.2499999999999999E-2</v>
       </c>
       <c r="H14" s="8">
-        <v>1.71</v>
+        <v>0.63</v>
       </c>
       <c r="I14" s="6">
-        <v>0.35</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="J14" s="8">
-        <v>30.687999999999999</v>
+        <v>28.687999999999999</v>
       </c>
       <c r="K14" s="8">
-        <v>37.456000000000003</v>
+        <v>31.456</v>
       </c>
       <c r="L14" s="8">
-        <v>31.856000000000002</v>
+        <v>39.856000000000002</v>
       </c>
       <c r="M14" s="4"/>
       <c r="N14" s="4"/>
@@ -1423,48 +1413,48 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="6">
-        <v>21.08</v>
+        <v>22.58</v>
       </c>
       <c r="U14" s="9">
-        <v>46.76</v>
+        <v>19.46</v>
       </c>
     </row>
     <row r="15" spans="1:21">
       <c r="A15" s="4">
-        <v>2408</v>
+        <v>2407</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="D15" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E15" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.17</v>
       </c>
       <c r="F15" s="6">
-        <v>7.81</v>
+        <v>7.2</v>
       </c>
       <c r="G15" s="7">
-        <v>2.2599999999999999E-2</v>
+        <v>6.6299999999999998E-2</v>
       </c>
       <c r="H15" s="8">
-        <v>0.65</v>
+        <v>1.71</v>
       </c>
       <c r="I15" s="6">
-        <v>1.2</v>
+        <v>0.35</v>
       </c>
       <c r="J15" s="8">
-        <v>24.687999999999999</v>
+        <v>30.687999999999999</v>
       </c>
       <c r="K15" s="8">
-        <v>27.456</v>
+        <v>37.456000000000003</v>
       </c>
       <c r="L15" s="8">
-        <v>47.856000000000002</v>
+        <v>31.856000000000002</v>
       </c>
       <c r="M15" s="4"/>
       <c r="N15" s="4"/>
@@ -1474,48 +1464,48 @@
       <c r="R15" s="4"/>
       <c r="S15" s="4"/>
       <c r="T15" s="6">
-        <v>14.67</v>
+        <v>21.08</v>
       </c>
       <c r="U15" s="9">
-        <v>33.32</v>
+        <v>46.76</v>
       </c>
     </row>
     <row r="16" spans="1:21">
       <c r="A16" s="4">
-        <v>2409</v>
+        <v>2408</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>27</v>
+        <v>54</v>
       </c>
       <c r="D16" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E16" s="4">
-        <v>0.39</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F16" s="6">
-        <v>7.71</v>
+        <v>7.81</v>
       </c>
       <c r="G16" s="7">
-        <v>2.5999999999999999E-2</v>
+        <v>2.2599999999999999E-2</v>
       </c>
       <c r="H16" s="8">
-        <v>0.71</v>
+        <v>0.65</v>
       </c>
       <c r="I16" s="6">
-        <v>4.8099999999999996</v>
+        <v>1.2</v>
       </c>
       <c r="J16" s="8">
-        <v>34.688000000000002</v>
+        <v>24.687999999999999</v>
       </c>
       <c r="K16" s="8">
-        <v>23.456</v>
+        <v>27.456</v>
       </c>
       <c r="L16" s="8">
-        <v>41.856000000000002</v>
+        <v>47.856000000000002</v>
       </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
@@ -1525,48 +1515,48 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="6">
-        <v>10.08</v>
+        <v>14.67</v>
       </c>
       <c r="U16" s="9">
-        <v>58.81</v>
+        <v>33.32</v>
       </c>
     </row>
     <row r="17" spans="1:21">
       <c r="A17" s="4">
-        <v>2410</v>
+        <v>2409</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>57</v>
+        <v>27</v>
       </c>
       <c r="D17" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E17" s="4">
-        <v>0.56000000000000005</v>
+        <v>0.39</v>
       </c>
       <c r="F17" s="6">
-        <v>7.73</v>
+        <v>7.71</v>
       </c>
       <c r="G17" s="7">
-        <v>2.9600000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="H17" s="8">
-        <v>0.74</v>
+        <v>0.71</v>
       </c>
       <c r="I17" s="6">
-        <v>2.19</v>
+        <v>4.8099999999999996</v>
       </c>
       <c r="J17" s="8">
-        <v>32.688000000000002</v>
+        <v>34.688000000000002</v>
       </c>
       <c r="K17" s="8">
-        <v>33.456000000000003</v>
+        <v>23.456</v>
       </c>
       <c r="L17" s="8">
-        <v>33.856000000000002</v>
+        <v>41.856000000000002</v>
       </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -1576,48 +1566,48 @@
       <c r="R17" s="4"/>
       <c r="S17" s="4"/>
       <c r="T17" s="6">
-        <v>5.83</v>
-      </c>
-      <c r="U17" s="6">
-        <v>33.89</v>
+        <v>10.08</v>
+      </c>
+      <c r="U17" s="9">
+        <v>58.81</v>
       </c>
     </row>
     <row r="18" spans="1:21">
       <c r="A18" s="4">
-        <v>2411</v>
+        <v>2410</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E18" s="4">
-        <v>0.39</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="F18" s="6">
-        <v>7.65</v>
+        <v>7.73</v>
       </c>
       <c r="G18" s="7">
-        <v>4.8599999999999997E-2</v>
+        <v>2.9600000000000001E-2</v>
       </c>
       <c r="H18" s="8">
-        <v>1.21</v>
+        <v>0.74</v>
       </c>
       <c r="I18" s="6">
-        <v>8.41</v>
+        <v>2.19</v>
       </c>
       <c r="J18" s="8">
-        <v>20.687999999999999</v>
+        <v>32.688000000000002</v>
       </c>
       <c r="K18" s="8">
-        <v>39.456000000000003</v>
+        <v>33.456000000000003</v>
       </c>
       <c r="L18" s="8">
-        <v>39.856000000000002</v>
+        <v>33.856000000000002</v>
       </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
@@ -1627,21 +1617,21 @@
       <c r="R18" s="4"/>
       <c r="S18" s="4"/>
       <c r="T18" s="6">
-        <v>9.33</v>
+        <v>5.83</v>
       </c>
       <c r="U18" s="6">
-        <v>56.19</v>
+        <v>33.89</v>
       </c>
     </row>
     <row r="19" spans="1:21">
       <c r="A19" s="4">
-        <v>2412</v>
+        <v>2411</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D19" s="10" t="s">
         <v>68</v>
@@ -1650,25 +1640,25 @@
         <v>0.39</v>
       </c>
       <c r="F19" s="6">
-        <v>7.49</v>
+        <v>7.65</v>
       </c>
       <c r="G19" s="7">
-        <v>4.1399999999999999E-2</v>
+        <v>4.8599999999999997E-2</v>
       </c>
       <c r="H19" s="8">
-        <v>1.0900000000000001</v>
+        <v>1.21</v>
       </c>
       <c r="I19" s="6">
-        <v>1.1299999999999999</v>
+        <v>8.41</v>
       </c>
       <c r="J19" s="8">
-        <v>18.687999999999999</v>
+        <v>20.687999999999999</v>
       </c>
       <c r="K19" s="8">
-        <v>35.456000000000003</v>
+        <v>39.456000000000003</v>
       </c>
       <c r="L19" s="8">
-        <v>45.856000000000002</v>
+        <v>39.856000000000002</v>
       </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
@@ -1678,21 +1668,21 @@
       <c r="R19" s="4"/>
       <c r="S19" s="4"/>
       <c r="T19" s="6">
-        <v>10.67</v>
+        <v>9.33</v>
       </c>
       <c r="U19" s="6">
-        <v>39.92</v>
+        <v>56.19</v>
       </c>
     </row>
     <row r="20" spans="1:21">
       <c r="A20" s="4">
-        <v>2413</v>
+        <v>2412</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D20" s="10" t="s">
         <v>68</v>
@@ -1701,25 +1691,25 @@
         <v>0.39</v>
       </c>
       <c r="F20" s="6">
-        <v>7.71</v>
+        <v>7.49</v>
       </c>
       <c r="G20" s="7">
-        <v>4.41E-2</v>
+        <v>4.1399999999999999E-2</v>
       </c>
       <c r="H20" s="8">
-        <v>1.08</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I20" s="6">
-        <v>6.86</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="J20" s="8">
-        <v>22.687999999999999</v>
+        <v>18.687999999999999</v>
       </c>
       <c r="K20" s="8">
-        <v>39.456000000000003</v>
+        <v>35.456000000000003</v>
       </c>
       <c r="L20" s="8">
-        <v>37.856000000000002</v>
+        <v>45.856000000000002</v>
       </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -1729,48 +1719,48 @@
       <c r="R20" s="4"/>
       <c r="S20" s="4"/>
       <c r="T20" s="6">
-        <v>8.42</v>
+        <v>10.67</v>
       </c>
       <c r="U20" s="6">
-        <v>50.16</v>
+        <v>39.92</v>
       </c>
     </row>
     <row r="21" spans="1:21">
       <c r="A21" s="4">
-        <v>2414</v>
+        <v>2413</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>34</v>
+        <v>60</v>
       </c>
       <c r="D21" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E21" s="4">
-        <v>0.45</v>
+        <v>0.39</v>
       </c>
       <c r="F21" s="6">
-        <v>7.6</v>
+        <v>7.71</v>
       </c>
       <c r="G21" s="7">
-        <v>4.5999999999999999E-2</v>
+        <v>4.41E-2</v>
       </c>
       <c r="H21" s="8">
-        <v>1.21</v>
+        <v>1.08</v>
       </c>
       <c r="I21" s="6">
-        <v>0.56999999999999995</v>
+        <v>6.86</v>
       </c>
       <c r="J21" s="8">
-        <v>26.687999999999999</v>
+        <v>22.687999999999999</v>
       </c>
       <c r="K21" s="8">
-        <v>31.456</v>
+        <v>39.456000000000003</v>
       </c>
       <c r="L21" s="8">
-        <v>41.856000000000002</v>
+        <v>37.856000000000002</v>
       </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
@@ -1780,48 +1770,48 @@
       <c r="R21" s="4"/>
       <c r="S21" s="4"/>
       <c r="T21" s="6">
-        <v>14.17</v>
+        <v>8.42</v>
       </c>
       <c r="U21" s="6">
-        <v>78.209999999999994</v>
+        <v>50.16</v>
       </c>
     </row>
     <row r="22" spans="1:21">
       <c r="A22" s="4">
-        <v>2415</v>
+        <v>2414</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D22" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E22" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.45</v>
       </c>
       <c r="F22" s="6">
-        <v>7.71</v>
+        <v>7.6</v>
       </c>
       <c r="G22" s="7">
-        <v>1.7100000000000001E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="H22" s="8">
-        <v>0.54</v>
+        <v>1.21</v>
       </c>
       <c r="I22" s="6">
-        <v>5.37</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J22" s="8">
-        <v>40.688000000000002</v>
+        <v>26.687999999999999</v>
       </c>
       <c r="K22" s="8">
-        <v>35.456000000000003</v>
+        <v>31.456</v>
       </c>
       <c r="L22" s="8">
-        <v>23.856000000000002</v>
+        <v>41.856000000000002</v>
       </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
@@ -1831,48 +1821,48 @@
       <c r="R22" s="4"/>
       <c r="S22" s="4"/>
       <c r="T22" s="6">
-        <v>16.670000000000002</v>
+        <v>14.17</v>
       </c>
       <c r="U22" s="6">
-        <v>67.849999999999994</v>
+        <v>78.209999999999994</v>
       </c>
     </row>
     <row r="23" spans="1:21">
       <c r="A23" s="4">
-        <v>2416</v>
+        <v>2415</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="D23" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E23" s="4">
-        <v>0.39</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F23" s="6">
-        <v>7.51</v>
+        <v>7.71</v>
       </c>
       <c r="G23" s="7">
-        <v>4.2299999999999997E-2</v>
+        <v>1.7100000000000001E-2</v>
       </c>
       <c r="H23" s="8">
-        <v>1.21</v>
+        <v>0.54</v>
       </c>
       <c r="I23" s="6">
-        <v>7.7</v>
+        <v>5.37</v>
       </c>
       <c r="J23" s="8">
-        <v>48.688000000000002</v>
+        <v>40.688000000000002</v>
       </c>
       <c r="K23" s="8">
         <v>35.456000000000003</v>
       </c>
       <c r="L23" s="8">
-        <v>15.856</v>
+        <v>23.856000000000002</v>
       </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
@@ -1882,21 +1872,21 @@
       <c r="R23" s="4"/>
       <c r="S23" s="4"/>
       <c r="T23" s="6">
-        <v>18.170000000000002</v>
+        <v>16.670000000000002</v>
       </c>
       <c r="U23" s="6">
-        <v>79.3</v>
+        <v>67.849999999999994</v>
       </c>
     </row>
     <row r="24" spans="1:21">
       <c r="A24" s="4">
-        <v>2417</v>
+        <v>2416</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D24" s="10" t="s">
         <v>68</v>
@@ -1905,25 +1895,25 @@
         <v>0.39</v>
       </c>
       <c r="F24" s="6">
+        <v>7.51</v>
+      </c>
+      <c r="G24" s="7">
+        <v>4.2299999999999997E-2</v>
+      </c>
+      <c r="H24" s="8">
+        <v>1.21</v>
+      </c>
+      <c r="I24" s="6">
         <v>7.7</v>
       </c>
-      <c r="G24" s="7">
-        <v>3.4799999999999998E-2</v>
-      </c>
-      <c r="H24" s="8">
-        <v>0.95</v>
-      </c>
-      <c r="I24" s="6">
-        <v>9.0500000000000007</v>
-      </c>
       <c r="J24" s="8">
-        <v>34.688000000000002</v>
+        <v>48.688000000000002</v>
       </c>
       <c r="K24" s="8">
-        <v>33.456000000000003</v>
+        <v>35.456000000000003</v>
       </c>
       <c r="L24" s="8">
-        <v>31.856000000000002</v>
+        <v>15.856</v>
       </c>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
@@ -1933,48 +1923,48 @@
       <c r="R24" s="4"/>
       <c r="S24" s="4"/>
       <c r="T24" s="6">
-        <v>9.08</v>
+        <v>18.170000000000002</v>
       </c>
       <c r="U24" s="6">
-        <v>60.44</v>
+        <v>79.3</v>
       </c>
     </row>
     <row r="25" spans="1:21">
       <c r="A25" s="4">
-        <v>2418</v>
+        <v>2417</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C25" s="10" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="D25" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E25" s="4">
-        <v>0.17</v>
+        <v>0.39</v>
       </c>
       <c r="F25" s="6">
-        <v>7.43</v>
+        <v>7.7</v>
       </c>
       <c r="G25" s="7">
-        <v>4.3200000000000002E-2</v>
+        <v>3.4799999999999998E-2</v>
       </c>
       <c r="H25" s="8">
-        <v>1.33</v>
+        <v>0.95</v>
       </c>
       <c r="I25" s="6">
-        <v>7.21</v>
+        <v>9.0500000000000007</v>
       </c>
       <c r="J25" s="8">
-        <v>66.688000000000002</v>
+        <v>34.688000000000002</v>
       </c>
       <c r="K25" s="8">
-        <v>15.456</v>
+        <v>33.456000000000003</v>
       </c>
       <c r="L25" s="8">
-        <v>17.856000000000002</v>
+        <v>31.856000000000002</v>
       </c>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
@@ -1984,21 +1974,21 @@
       <c r="R25" s="4"/>
       <c r="S25" s="4"/>
       <c r="T25" s="6">
-        <v>8</v>
+        <v>9.08</v>
       </c>
       <c r="U25" s="6">
-        <v>26.07</v>
+        <v>60.44</v>
       </c>
     </row>
     <row r="26" spans="1:21">
       <c r="A26" s="4">
-        <v>2419</v>
+        <v>2418</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>68</v>
@@ -2007,25 +1997,25 @@
         <v>0.17</v>
       </c>
       <c r="F26" s="6">
-        <v>7.74</v>
+        <v>7.43</v>
       </c>
       <c r="G26" s="7">
-        <v>1.12E-2</v>
+        <v>4.3200000000000002E-2</v>
       </c>
       <c r="H26" s="8">
-        <v>0.3</v>
+        <v>1.33</v>
       </c>
       <c r="I26" s="6">
-        <v>0.28000000000000003</v>
+        <v>7.21</v>
       </c>
       <c r="J26" s="8">
-        <v>36.688000000000002</v>
+        <v>66.688000000000002</v>
       </c>
       <c r="K26" s="8">
-        <v>23.456</v>
+        <v>15.456</v>
       </c>
       <c r="L26" s="8">
-        <v>39.856000000000002</v>
+        <v>17.856000000000002</v>
       </c>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
@@ -2035,21 +2025,21 @@
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
       <c r="T26" s="6">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="U26" s="6">
-        <v>32.090000000000003</v>
+        <v>26.07</v>
       </c>
     </row>
     <row r="27" spans="1:21">
       <c r="A27" s="4">
-        <v>3611</v>
+        <v>2419</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>63</v>
+        <v>35</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>39</v>
+        <v>62</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>68</v>
@@ -2057,526 +2047,544 @@
       <c r="E27" s="4">
         <v>0.17</v>
       </c>
-      <c r="F27" s="16">
-        <v>7.98</v>
-      </c>
-      <c r="G27" s="17">
-        <v>3.7131494399999999E-2</v>
-      </c>
-      <c r="H27" s="17">
-        <v>1.0920000000000001</v>
-      </c>
-      <c r="I27" s="18">
-        <v>24.3386</v>
-      </c>
-      <c r="J27" s="16">
-        <v>35.768000000000001</v>
-      </c>
-      <c r="K27" s="16">
-        <v>35.024000000000001</v>
-      </c>
-      <c r="L27" s="16">
-        <v>29.207999999999998</v>
-      </c>
-      <c r="M27" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="N27" s="17">
-        <v>1.6359612500000003</v>
-      </c>
-      <c r="O27" s="17">
-        <v>2.2088797500000004</v>
-      </c>
-      <c r="P27" s="17">
-        <v>7.5168324000000011</v>
-      </c>
-      <c r="Q27" s="17">
-        <v>6.3113812627006398</v>
-      </c>
-      <c r="R27" s="17">
-        <v>5.4213902771036828</v>
-      </c>
-      <c r="S27" s="16">
-        <v>1.3813799999999998E-2</v>
-      </c>
-      <c r="T27" s="13"/>
-      <c r="U27" s="13"/>
+      <c r="F27" s="6">
+        <v>7.74</v>
+      </c>
+      <c r="G27" s="7">
+        <v>1.12E-2</v>
+      </c>
+      <c r="H27" s="8">
+        <v>0.3</v>
+      </c>
+      <c r="I27" s="6">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J27" s="8">
+        <v>36.688000000000002</v>
+      </c>
+      <c r="K27" s="8">
+        <v>23.456</v>
+      </c>
+      <c r="L27" s="8">
+        <v>39.856000000000002</v>
+      </c>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="6">
+        <v>10</v>
+      </c>
+      <c r="U27" s="6">
+        <v>32.090000000000003</v>
+      </c>
     </row>
     <row r="28" spans="1:21">
       <c r="A28" s="4">
-        <v>3613</v>
+        <v>3611</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E28" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.17</v>
       </c>
       <c r="F28" s="16">
-        <v>8.02</v>
+        <v>7.98</v>
       </c>
       <c r="G28" s="17">
-        <v>2.4939340800000001E-2</v>
+        <v>3.7131494399999999E-2</v>
       </c>
       <c r="H28" s="17">
-        <v>0.63600000000000001</v>
+        <v>1.0920000000000001</v>
       </c>
       <c r="I28" s="18">
-        <v>18.470399999999998</v>
+        <v>24.3386</v>
       </c>
       <c r="J28" s="16">
-        <v>23.768000000000001</v>
+        <v>35.768000000000001</v>
       </c>
       <c r="K28" s="16">
-        <v>37.024000000000001</v>
+        <v>35.024000000000001</v>
       </c>
       <c r="L28" s="16">
-        <v>39.207999999999998</v>
+        <v>29.207999999999998</v>
       </c>
       <c r="M28" s="19" t="s">
         <v>2</v>
       </c>
       <c r="N28" s="17">
-        <v>0.43920378333333338</v>
+        <v>1.6359612500000003</v>
       </c>
       <c r="O28" s="17">
-        <v>1.11051875</v>
+        <v>2.2088797500000004</v>
       </c>
       <c r="P28" s="17">
-        <v>3.7430109391304351</v>
+        <v>7.5168324000000011</v>
       </c>
       <c r="Q28" s="17">
-        <v>4.7727235820757681</v>
+        <v>6.3113812627006398</v>
       </c>
       <c r="R28" s="17">
-        <v>4.2521553249873225</v>
+        <v>5.4213902771036828</v>
       </c>
       <c r="S28" s="16">
-        <v>1.71556E-2</v>
+        <v>1.3813799999999998E-2</v>
       </c>
       <c r="T28" s="13"/>
       <c r="U28" s="13"/>
     </row>
     <row r="29" spans="1:21">
       <c r="A29" s="4">
-        <v>3614</v>
+        <v>3613</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="D29" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E29" s="4">
-        <v>0.22</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F29" s="16">
-        <v>7.99</v>
+        <v>8.02</v>
       </c>
       <c r="G29" s="17">
-        <v>2.2169100799999997E-2</v>
+        <v>2.4939340800000001E-2</v>
       </c>
       <c r="H29" s="17">
-        <v>0.58099999999999996</v>
+        <v>0.63600000000000001</v>
       </c>
       <c r="I29" s="18">
-        <v>19.432399999999998</v>
+        <v>18.470399999999998</v>
       </c>
       <c r="J29" s="16">
-        <v>25.768000000000001</v>
+        <v>23.768000000000001</v>
       </c>
       <c r="K29" s="16">
-        <v>39.024000000000001</v>
+        <v>37.024000000000001</v>
       </c>
       <c r="L29" s="16">
-        <v>35.207999999999998</v>
+        <v>39.207999999999998</v>
       </c>
       <c r="M29" s="19" t="s">
         <v>2</v>
       </c>
       <c r="N29" s="17">
-        <v>0.52614650000000007</v>
+        <v>0.43920378333333338</v>
       </c>
       <c r="O29" s="17">
-        <v>0.74763480000000004</v>
+        <v>1.11051875</v>
       </c>
       <c r="P29" s="17">
-        <v>2.2262004313043477</v>
+        <v>3.7430109391304351</v>
       </c>
       <c r="Q29" s="17">
-        <v>2.775340357377333</v>
+        <v>4.7727235820757681</v>
       </c>
       <c r="R29" s="17">
-        <v>2.789535071521001</v>
+        <v>4.2521553249873225</v>
       </c>
       <c r="S29" s="16">
-        <v>0.21224720000000002</v>
+        <v>1.71556E-2</v>
       </c>
       <c r="T29" s="13"/>
       <c r="U29" s="13"/>
     </row>
     <row r="30" spans="1:21">
       <c r="A30" s="4">
-        <v>3623</v>
+        <v>3614</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="D30" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E30" s="4">
-        <v>0.45</v>
+        <v>0.22</v>
       </c>
       <c r="F30" s="16">
-        <v>7.89</v>
+        <v>7.99</v>
       </c>
       <c r="G30" s="17">
-        <v>3.4190956799999991E-2</v>
+        <v>2.2169100799999997E-2</v>
       </c>
       <c r="H30" s="17">
-        <v>0.81899999999999995</v>
+        <v>0.58099999999999996</v>
       </c>
       <c r="I30" s="18">
-        <v>18.662799999999997</v>
+        <v>19.432399999999998</v>
       </c>
       <c r="J30" s="16">
-        <v>33.768000000000001</v>
+        <v>25.768000000000001</v>
       </c>
       <c r="K30" s="16">
-        <v>43.023999999999994</v>
+        <v>39.024000000000001</v>
       </c>
       <c r="L30" s="16">
-        <v>23.208000000000006</v>
+        <v>35.207999999999998</v>
       </c>
       <c r="M30" s="19" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="N30" s="17">
-        <v>2.0498527499999999</v>
+        <v>0.52614650000000007</v>
       </c>
       <c r="O30" s="17">
-        <v>2.4731954499999995</v>
+        <v>0.74763480000000004</v>
       </c>
       <c r="P30" s="17">
-        <v>4.4076194608695651</v>
+        <v>2.2262004313043477</v>
       </c>
       <c r="Q30" s="17">
-        <v>2.9720648133507872</v>
+        <v>2.775340357377333</v>
       </c>
       <c r="R30" s="17">
-        <v>2.9309167429915104</v>
+        <v>2.789535071521001</v>
       </c>
       <c r="S30" s="16">
-        <v>3.9790299999999994E-2</v>
+        <v>0.21224720000000002</v>
       </c>
       <c r="T30" s="13"/>
       <c r="U30" s="13"/>
     </row>
     <row r="31" spans="1:21">
       <c r="A31" s="4">
-        <v>3626</v>
+        <v>3623</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D31" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E31" s="4">
-        <v>0.34</v>
+        <v>0.45</v>
       </c>
       <c r="F31" s="16">
-        <v>8.24</v>
+        <v>7.89</v>
       </c>
       <c r="G31" s="17">
-        <v>2.9607564799999996E-2</v>
+        <v>3.4190956799999991E-2</v>
       </c>
       <c r="H31" s="17">
-        <v>0.878</v>
+        <v>0.81899999999999995</v>
       </c>
       <c r="I31" s="18">
-        <v>25.492999999999999</v>
+        <v>18.662799999999997</v>
       </c>
       <c r="J31" s="16">
-        <v>39.768000000000001</v>
+        <v>33.768000000000001</v>
       </c>
       <c r="K31" s="16">
-        <v>29.024000000000001</v>
+        <v>43.023999999999994</v>
       </c>
       <c r="L31" s="16">
-        <v>31.207999999999998</v>
+        <v>23.208000000000006</v>
       </c>
       <c r="M31" s="19" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="N31" s="17">
-        <v>0.86543324999999982</v>
+        <v>2.0498527499999999</v>
       </c>
       <c r="O31" s="17">
-        <v>1.0445792499999997</v>
+        <v>2.4731954499999995</v>
       </c>
       <c r="P31" s="17">
-        <v>6.6801756521739124</v>
+        <v>4.4076194608695651</v>
       </c>
       <c r="Q31" s="17">
-        <v>8.1074067611585914</v>
+        <v>2.9720648133507872</v>
       </c>
       <c r="R31" s="17">
-        <v>6.8357280296487986</v>
+        <v>2.9309167429915104</v>
       </c>
       <c r="S31" s="16">
-        <v>0.76716640000000003</v>
+        <v>3.9790299999999994E-2</v>
       </c>
       <c r="T31" s="13"/>
       <c r="U31" s="13"/>
     </row>
     <row r="32" spans="1:21">
       <c r="A32" s="4">
-        <v>3627</v>
+        <v>3626</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="D32" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E32" s="4">
-        <v>0.28000000000000003</v>
+        <v>0.34</v>
       </c>
       <c r="F32" s="16">
-        <v>8.2200000000000006</v>
+        <v>8.24</v>
       </c>
       <c r="G32" s="17">
-        <v>4.5720575999999999E-2</v>
+        <v>2.9607564799999996E-2</v>
       </c>
       <c r="H32" s="17">
-        <v>0.98399999999999999</v>
+        <v>0.878</v>
       </c>
       <c r="I32" s="18">
-        <v>26.0702</v>
+        <v>25.492999999999999</v>
       </c>
       <c r="J32" s="16">
-        <v>47.768000000000001</v>
+        <v>39.768000000000001</v>
       </c>
       <c r="K32" s="16">
-        <v>33.024000000000001</v>
+        <v>29.024000000000001</v>
       </c>
       <c r="L32" s="16">
-        <v>19.207999999999998</v>
+        <v>31.207999999999998</v>
       </c>
       <c r="M32" s="19" t="s">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="N32" s="17">
-        <v>1.38303</v>
+        <v>0.86543324999999982</v>
       </c>
       <c r="O32" s="17">
-        <v>1.8012059999999999</v>
+        <v>1.0445792499999997</v>
       </c>
       <c r="P32" s="17">
-        <v>10.220312347826086</v>
+        <v>6.6801756521739124</v>
       </c>
       <c r="Q32" s="17">
-        <v>9.6553715013538604</v>
+        <v>8.1074067611585914</v>
       </c>
       <c r="R32" s="17">
-        <v>8.0998419089871305</v>
+        <v>6.8357280296487986</v>
       </c>
       <c r="S32" s="16">
-        <v>1.2341999999999995E-2</v>
+        <v>0.76716640000000003</v>
       </c>
       <c r="T32" s="13"/>
       <c r="U32" s="13"/>
     </row>
     <row r="33" spans="1:21">
       <c r="A33" s="4">
-        <v>3630</v>
+        <v>3627</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="D33" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E33" s="4">
-        <v>0.5</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="F33" s="16">
-        <v>7.76</v>
+        <v>8.2200000000000006</v>
       </c>
       <c r="G33" s="17">
-        <v>1.2528172799999999E-2</v>
+        <v>4.5720575999999999E-2</v>
       </c>
       <c r="H33" s="17">
-        <v>0.35099999999999998</v>
+        <v>0.98399999999999999</v>
       </c>
       <c r="I33" s="18">
-        <v>43.097599999999993</v>
+        <v>26.0702</v>
       </c>
       <c r="J33" s="16">
-        <v>47.695999999999998</v>
+        <v>47.768000000000001</v>
       </c>
       <c r="K33" s="16">
-        <v>40.951999999999998</v>
+        <v>33.024000000000001</v>
       </c>
       <c r="L33" s="16">
-        <v>11.352000000000004</v>
+        <v>19.207999999999998</v>
       </c>
       <c r="M33" s="19" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N33" s="17">
-        <v>0.47311550000000002</v>
+        <v>1.38303</v>
       </c>
       <c r="O33" s="17">
-        <v>0.91908960000000017</v>
+        <v>1.8012059999999999</v>
       </c>
       <c r="P33" s="17">
-        <v>0.57455708869565236</v>
+        <v>10.220312347826086</v>
       </c>
       <c r="Q33" s="17">
-        <v>0.24484389497644701</v>
+        <v>9.6553715013538604</v>
       </c>
       <c r="R33" s="17">
-        <v>0.68864686517589468</v>
+        <v>8.0998419089871305</v>
       </c>
       <c r="S33" s="16">
-        <v>4.9635300000000007E-2</v>
+        <v>1.2341999999999995E-2</v>
       </c>
       <c r="T33" s="13"/>
       <c r="U33" s="13"/>
     </row>
     <row r="34" spans="1:21">
       <c r="A34" s="4">
-        <v>3631</v>
+        <v>3630</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D34" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E34" s="4">
-        <v>0.39</v>
+        <v>0.5</v>
       </c>
       <c r="F34" s="16">
-        <v>7.79</v>
+        <v>7.76</v>
       </c>
       <c r="G34" s="17">
-        <v>1.45112E-2</v>
+        <v>1.2528172799999999E-2</v>
       </c>
       <c r="H34" s="17">
-        <v>0.42499999999999999</v>
+        <v>0.35099999999999998</v>
       </c>
       <c r="I34" s="18">
-        <v>15.488200000000001</v>
+        <v>43.097599999999993</v>
       </c>
       <c r="J34" s="16">
-        <v>43.695999999999998</v>
+        <v>47.695999999999998</v>
       </c>
       <c r="K34" s="16">
-        <v>42.951999999999998</v>
+        <v>40.951999999999998</v>
       </c>
       <c r="L34" s="16">
-        <v>13.352000000000004</v>
+        <v>11.352000000000004</v>
       </c>
       <c r="M34" s="19" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="N34" s="17">
-        <v>0.45480874999999998</v>
+        <v>0.47311550000000002</v>
       </c>
       <c r="O34" s="17">
-        <v>0.79598199999999997</v>
+        <v>0.91908960000000017</v>
       </c>
       <c r="P34" s="17">
-        <v>0.76606888695652164</v>
+        <v>0.57455708869565236</v>
       </c>
       <c r="Q34" s="17">
-        <v>0.16855184473830379</v>
+        <v>0.24484389497644701</v>
       </c>
       <c r="R34" s="17">
-        <v>0.96870265874004802</v>
+        <v>0.68864686517589468</v>
       </c>
       <c r="S34" s="16">
-        <v>5.9218499999999993E-2</v>
+        <v>4.9635300000000007E-2</v>
       </c>
       <c r="T34" s="13"/>
       <c r="U34" s="13"/>
     </row>
     <row r="35" spans="1:21">
       <c r="A35" s="4">
-        <v>3633</v>
+        <v>3631</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="D35" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E35" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-      <c r="H35" s="4"/>
-      <c r="I35" s="4"/>
-      <c r="J35" s="4"/>
-      <c r="K35" s="4"/>
-      <c r="L35" s="4"/>
-      <c r="M35" s="4"/>
-      <c r="N35" s="4"/>
-      <c r="O35" s="4"/>
-      <c r="P35" s="4"/>
-      <c r="Q35" s="4"/>
-      <c r="R35" s="4"/>
-      <c r="S35" s="4"/>
+        <v>0.39</v>
+      </c>
+      <c r="F35" s="16">
+        <v>7.79</v>
+      </c>
+      <c r="G35" s="17">
+        <v>1.45112E-2</v>
+      </c>
+      <c r="H35" s="17">
+        <v>0.42499999999999999</v>
+      </c>
+      <c r="I35" s="18">
+        <v>15.488200000000001</v>
+      </c>
+      <c r="J35" s="16">
+        <v>43.695999999999998</v>
+      </c>
+      <c r="K35" s="16">
+        <v>42.951999999999998</v>
+      </c>
+      <c r="L35" s="16">
+        <v>13.352000000000004</v>
+      </c>
+      <c r="M35" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="N35" s="17">
+        <v>0.45480874999999998</v>
+      </c>
+      <c r="O35" s="17">
+        <v>0.79598199999999997</v>
+      </c>
+      <c r="P35" s="17">
+        <v>0.76606888695652164</v>
+      </c>
+      <c r="Q35" s="17">
+        <v>0.16855184473830379</v>
+      </c>
+      <c r="R35" s="17">
+        <v>0.96870265874004802</v>
+      </c>
+      <c r="S35" s="16">
+        <v>5.9218499999999993E-2</v>
+      </c>
       <c r="T35" s="13"/>
       <c r="U35" s="13"/>
     </row>
     <row r="36" spans="1:21">
       <c r="A36" s="4">
-        <v>3634</v>
+        <v>3633</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="D36" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E36" s="4">
-        <v>0.34</v>
+        <v>0.17</v>
       </c>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
@@ -2595,48 +2603,48 @@
       <c r="T36" s="13"/>
       <c r="U36" s="13"/>
     </row>
-    <row r="37" spans="1:21" s="15" customFormat="1">
-      <c r="A37" s="14">
-        <v>12062</v>
-      </c>
-      <c r="B37" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C37" s="12">
-        <v>50</v>
-      </c>
-      <c r="D37" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="14">
-        <v>0.22</v>
-      </c>
-      <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="14"/>
-      <c r="I37" s="14"/>
-      <c r="J37" s="14"/>
-      <c r="K37" s="14"/>
-      <c r="L37" s="14"/>
-      <c r="M37" s="14"/>
-      <c r="N37" s="14"/>
-      <c r="O37" s="14"/>
-      <c r="P37" s="14"/>
-      <c r="Q37" s="14"/>
-      <c r="R37" s="14"/>
-      <c r="S37" s="14"/>
-      <c r="T37" s="14"/>
-      <c r="U37" s="14"/>
+    <row r="37" spans="1:21">
+      <c r="A37" s="4">
+        <v>3634</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="4">
+        <v>0.34</v>
+      </c>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="4"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="O37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="4"/>
+      <c r="R37" s="4"/>
+      <c r="S37" s="4"/>
+      <c r="T37" s="13"/>
+      <c r="U37" s="13"/>
     </row>
     <row r="38" spans="1:21" s="15" customFormat="1">
       <c r="A38" s="14">
-        <v>12631</v>
+        <v>12062</v>
       </c>
       <c r="B38" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C38" s="12" t="s">
-        <v>24</v>
+      <c r="C38" s="12">
+        <v>50</v>
       </c>
       <c r="D38" s="12" t="s">
         <v>67</v>
@@ -2661,54 +2669,54 @@
       <c r="T38" s="14"/>
       <c r="U38" s="14"/>
     </row>
-    <row r="39" spans="1:21">
-      <c r="A39" s="4">
-        <v>12636</v>
-      </c>
-      <c r="B39" s="4" t="s">
+    <row r="39" spans="1:21" s="27" customFormat="1">
+      <c r="A39" s="13">
+        <v>12631</v>
+      </c>
+      <c r="B39" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C39" s="10">
-        <v>41</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E39" s="4">
-        <v>0.84</v>
-      </c>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
-      <c r="H39" s="4"/>
-      <c r="I39" s="4"/>
-      <c r="J39" s="4"/>
-      <c r="K39" s="4"/>
-      <c r="L39" s="4"/>
-      <c r="M39" s="4"/>
-      <c r="N39" s="4"/>
-      <c r="O39" s="4"/>
-      <c r="P39" s="4"/>
-      <c r="Q39" s="4"/>
-      <c r="R39" s="4"/>
-      <c r="S39" s="4"/>
+      <c r="C39" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" s="13">
+        <v>0.22</v>
+      </c>
+      <c r="F39" s="13"/>
+      <c r="G39" s="13"/>
+      <c r="H39" s="13"/>
+      <c r="I39" s="13"/>
+      <c r="J39" s="13"/>
+      <c r="K39" s="13"/>
+      <c r="L39" s="13"/>
+      <c r="M39" s="13"/>
+      <c r="N39" s="13"/>
+      <c r="O39" s="13"/>
+      <c r="P39" s="13"/>
+      <c r="Q39" s="13"/>
+      <c r="R39" s="13"/>
+      <c r="S39" s="13"/>
       <c r="T39" s="13"/>
       <c r="U39" s="13"/>
     </row>
     <row r="40" spans="1:21">
       <c r="A40" s="4">
-        <v>12637</v>
+        <v>12636</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C40" s="10">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D40" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E40" s="4">
-        <v>0.22</v>
+        <v>0.84</v>
       </c>
       <c r="F40" s="4"/>
       <c r="G40" s="4"/>
@@ -2727,450 +2735,450 @@
       <c r="T40" s="13"/>
       <c r="U40" s="13"/>
     </row>
-    <row r="41" spans="1:21" s="15" customFormat="1">
-      <c r="A41" s="14">
+    <row r="41" spans="1:21">
+      <c r="A41" s="4">
+        <v>12637</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="10">
+        <v>42</v>
+      </c>
+      <c r="D41" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E41" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="F41" s="4"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="4"/>
+      <c r="L41" s="4"/>
+      <c r="M41" s="4"/>
+      <c r="N41" s="4"/>
+      <c r="O41" s="4"/>
+      <c r="P41" s="4"/>
+      <c r="Q41" s="4"/>
+      <c r="R41" s="4"/>
+      <c r="S41" s="4"/>
+      <c r="T41" s="13"/>
+      <c r="U41" s="13"/>
+    </row>
+    <row r="42" spans="1:21" s="25" customFormat="1">
+      <c r="A42" s="23">
         <v>12638</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B42" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C41" s="12">
+      <c r="C42" s="24">
         <v>35</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D42" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E42" s="23">
+        <v>0.17</v>
+      </c>
+      <c r="F42" s="23"/>
+      <c r="G42" s="23"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
+      <c r="J42" s="23"/>
+      <c r="K42" s="23"/>
+      <c r="L42" s="23"/>
+      <c r="M42" s="23"/>
+      <c r="N42" s="23"/>
+      <c r="O42" s="23"/>
+      <c r="P42" s="23"/>
+      <c r="Q42" s="23"/>
+      <c r="R42" s="23"/>
+      <c r="S42" s="23"/>
+      <c r="T42" s="23"/>
+      <c r="U42" s="23"/>
+    </row>
+    <row r="43" spans="1:21">
+      <c r="A43" s="4">
+        <v>12639</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="10">
+        <v>49</v>
+      </c>
+      <c r="D43" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E43" s="4">
+        <v>0.39</v>
+      </c>
+      <c r="F43" s="4"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="4"/>
+      <c r="L43" s="4"/>
+      <c r="M43" s="4"/>
+      <c r="N43" s="4"/>
+      <c r="O43" s="4"/>
+      <c r="P43" s="4"/>
+      <c r="Q43" s="4"/>
+      <c r="R43" s="4"/>
+      <c r="S43" s="4"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+    </row>
+    <row r="44" spans="1:21" s="25" customFormat="1">
+      <c r="A44" s="23">
+        <v>12642</v>
+      </c>
+      <c r="B44" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="24">
+        <v>28</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="F44" s="23"/>
+      <c r="G44" s="23"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
+      <c r="J44" s="23"/>
+      <c r="K44" s="23"/>
+      <c r="L44" s="23"/>
+      <c r="M44" s="23"/>
+      <c r="N44" s="23"/>
+      <c r="O44" s="23"/>
+      <c r="P44" s="23"/>
+      <c r="Q44" s="23"/>
+      <c r="R44" s="23"/>
+      <c r="S44" s="23"/>
+      <c r="T44" s="23"/>
+      <c r="U44" s="23"/>
+    </row>
+    <row r="45" spans="1:21">
+      <c r="A45" s="4">
+        <v>12643</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="10">
+        <v>37</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" s="4">
+        <v>0.84</v>
+      </c>
+      <c r="F45" s="4"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="4"/>
+      <c r="L45" s="4"/>
+      <c r="M45" s="4"/>
+      <c r="N45" s="4"/>
+      <c r="O45" s="4"/>
+      <c r="P45" s="4"/>
+      <c r="Q45" s="4"/>
+      <c r="R45" s="4"/>
+      <c r="S45" s="4"/>
+      <c r="T45" s="13"/>
+      <c r="U45" s="13"/>
+    </row>
+    <row r="46" spans="1:21" s="25" customFormat="1">
+      <c r="A46" s="23">
+        <v>12645</v>
+      </c>
+      <c r="B46" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="24">
+        <v>30</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E46" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="F46" s="23"/>
+      <c r="G46" s="23"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
+      <c r="J46" s="23"/>
+      <c r="K46" s="23"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="23"/>
+      <c r="N46" s="23"/>
+      <c r="O46" s="23"/>
+      <c r="P46" s="23"/>
+      <c r="Q46" s="23"/>
+      <c r="R46" s="23"/>
+      <c r="S46" s="23"/>
+      <c r="T46" s="23"/>
+      <c r="U46" s="23"/>
+    </row>
+    <row r="47" spans="1:21" s="15" customFormat="1">
+      <c r="A47" s="14">
+        <v>12647</v>
+      </c>
+      <c r="B47" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="12">
+        <v>44</v>
+      </c>
+      <c r="D47" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="14">
-        <v>0.17</v>
-      </c>
-      <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="14"/>
-      <c r="I41" s="14"/>
-      <c r="J41" s="14"/>
-      <c r="K41" s="14"/>
-      <c r="L41" s="14"/>
-      <c r="M41" s="14"/>
-      <c r="N41" s="14"/>
-      <c r="O41" s="14"/>
-      <c r="P41" s="14"/>
-      <c r="Q41" s="14"/>
-      <c r="R41" s="14"/>
-      <c r="S41" s="14"/>
-      <c r="T41" s="14"/>
-      <c r="U41" s="14"/>
-    </row>
-    <row r="42" spans="1:21">
-      <c r="A42" s="4">
-        <v>12639</v>
-      </c>
-      <c r="B42" s="4" t="s">
+      <c r="E47" s="14">
+        <v>0.22</v>
+      </c>
+      <c r="F47" s="14"/>
+      <c r="G47" s="14"/>
+      <c r="H47" s="14"/>
+      <c r="I47" s="14"/>
+      <c r="J47" s="14"/>
+      <c r="K47" s="14"/>
+      <c r="L47" s="14"/>
+      <c r="M47" s="14"/>
+      <c r="N47" s="14"/>
+      <c r="O47" s="14"/>
+      <c r="P47" s="14"/>
+      <c r="Q47" s="14"/>
+      <c r="R47" s="14"/>
+      <c r="S47" s="14"/>
+      <c r="T47" s="14"/>
+      <c r="U47" s="14"/>
+    </row>
+    <row r="48" spans="1:21">
+      <c r="A48" s="4">
+        <v>12648</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C42" s="10">
-        <v>49</v>
-      </c>
-      <c r="D42" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E42" s="4">
-        <v>0.39</v>
-      </c>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
-      <c r="H42" s="4"/>
-      <c r="I42" s="4"/>
-      <c r="J42" s="4"/>
-      <c r="K42" s="4"/>
-      <c r="L42" s="4"/>
-      <c r="M42" s="4"/>
-      <c r="N42" s="4"/>
-      <c r="O42" s="4"/>
-      <c r="P42" s="4"/>
-      <c r="Q42" s="4"/>
-      <c r="R42" s="4"/>
-      <c r="S42" s="4"/>
-      <c r="T42" s="13"/>
-      <c r="U42" s="13"/>
-    </row>
-    <row r="43" spans="1:21" s="15" customFormat="1">
-      <c r="A43" s="14">
-        <v>12642</v>
-      </c>
-      <c r="B43" s="14" t="s">
+      <c r="C48" s="10">
+        <v>43</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E48" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="4"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="4"/>
+      <c r="Q48" s="4"/>
+      <c r="R48" s="4"/>
+      <c r="S48" s="4"/>
+      <c r="T48" s="13"/>
+      <c r="U48" s="13"/>
+    </row>
+    <row r="49" spans="1:21" s="25" customFormat="1">
+      <c r="A49" s="23">
+        <v>12649</v>
+      </c>
+      <c r="B49" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C43" s="12">
-        <v>28</v>
-      </c>
-      <c r="D43" s="12" t="s">
+      <c r="C49" s="24">
+        <v>26</v>
+      </c>
+      <c r="D49" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E49" s="23">
+        <v>0.34</v>
+      </c>
+      <c r="F49" s="23"/>
+      <c r="G49" s="23"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
+      <c r="J49" s="23"/>
+      <c r="K49" s="23"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="23"/>
+      <c r="N49" s="23"/>
+      <c r="O49" s="23"/>
+      <c r="P49" s="23"/>
+      <c r="Q49" s="23"/>
+      <c r="R49" s="23"/>
+      <c r="S49" s="23"/>
+      <c r="T49" s="23"/>
+      <c r="U49" s="23"/>
+    </row>
+    <row r="50" spans="1:21" s="27" customFormat="1">
+      <c r="A50" s="13">
+        <v>12650</v>
+      </c>
+      <c r="B50" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C50" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D50" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="14">
+      <c r="E50" s="13">
         <v>0.22</v>
       </c>
-      <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="14"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14"/>
-      <c r="K43" s="14"/>
-      <c r="L43" s="14"/>
-      <c r="M43" s="14"/>
-      <c r="N43" s="14"/>
-      <c r="O43" s="14"/>
-      <c r="P43" s="14"/>
-      <c r="Q43" s="14"/>
-      <c r="R43" s="14"/>
-      <c r="S43" s="14"/>
-      <c r="T43" s="14"/>
-      <c r="U43" s="14"/>
-    </row>
-    <row r="44" spans="1:21">
-      <c r="A44" s="4">
-        <v>12643</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C44" s="10">
-        <v>37</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E44" s="4">
-        <v>0.84</v>
-      </c>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
-      <c r="H44" s="4"/>
-      <c r="I44" s="4"/>
-      <c r="J44" s="4"/>
-      <c r="K44" s="4"/>
-      <c r="L44" s="4"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="4"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="4"/>
-      <c r="Q44" s="4"/>
-      <c r="R44" s="4"/>
-      <c r="S44" s="4"/>
-      <c r="T44" s="13"/>
-      <c r="U44" s="13"/>
-    </row>
-    <row r="45" spans="1:21" s="15" customFormat="1">
-      <c r="A45" s="14">
-        <v>12645</v>
-      </c>
-      <c r="B45" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C45" s="12">
-        <v>30</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E45" s="14">
-        <v>0.22</v>
-      </c>
-      <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
-      <c r="I45" s="14"/>
-      <c r="J45" s="14"/>
-      <c r="K45" s="14"/>
-      <c r="L45" s="14"/>
-      <c r="M45" s="14"/>
-      <c r="N45" s="14"/>
-      <c r="O45" s="14"/>
-      <c r="P45" s="14"/>
-      <c r="Q45" s="14"/>
-      <c r="R45" s="14"/>
-      <c r="S45" s="14"/>
-      <c r="T45" s="14"/>
-      <c r="U45" s="14"/>
-    </row>
-    <row r="46" spans="1:21">
-      <c r="A46" s="4">
-        <v>12647</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="10">
-        <v>44</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E46" s="4">
-        <v>0.22</v>
-      </c>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="4"/>
-      <c r="N46" s="4"/>
-      <c r="O46" s="4"/>
-      <c r="P46" s="4"/>
-      <c r="Q46" s="4"/>
-      <c r="R46" s="4"/>
-      <c r="S46" s="4"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="13"/>
-    </row>
-    <row r="47" spans="1:21">
-      <c r="A47" s="4">
-        <v>12648</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C47" s="10">
-        <v>43</v>
-      </c>
-      <c r="D47" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E47" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="13"/>
-      <c r="U47" s="13"/>
-    </row>
-    <row r="48" spans="1:21" s="15" customFormat="1">
-      <c r="A48" s="14">
-        <v>12649</v>
-      </c>
-      <c r="B48" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C48" s="12">
-        <v>26</v>
-      </c>
-      <c r="D48" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E48" s="14">
-        <v>0.34</v>
-      </c>
-      <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="14"/>
-      <c r="I48" s="14"/>
-      <c r="J48" s="14"/>
-      <c r="K48" s="14"/>
-      <c r="L48" s="14"/>
-      <c r="M48" s="14"/>
-      <c r="N48" s="14"/>
-      <c r="O48" s="14"/>
-      <c r="P48" s="14"/>
-      <c r="Q48" s="14"/>
-      <c r="R48" s="14"/>
-      <c r="S48" s="14"/>
-      <c r="T48" s="14"/>
-      <c r="U48" s="14"/>
-    </row>
-    <row r="49" spans="1:21" s="15" customFormat="1">
-      <c r="A49" s="14">
-        <v>12650</v>
-      </c>
-      <c r="B49" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C49" s="12" t="s">
-        <v>23</v>
-      </c>
-      <c r="D49" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E49" s="14">
-        <v>0.22</v>
-      </c>
-      <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="14"/>
-      <c r="I49" s="14"/>
-      <c r="J49" s="14"/>
-      <c r="K49" s="14"/>
-      <c r="L49" s="14"/>
-      <c r="M49" s="14"/>
-      <c r="N49" s="14"/>
-      <c r="O49" s="14"/>
-      <c r="P49" s="14"/>
-      <c r="Q49" s="14"/>
-      <c r="R49" s="14"/>
-      <c r="S49" s="14"/>
-      <c r="T49" s="14"/>
-      <c r="U49" s="14"/>
-    </row>
-    <row r="50" spans="1:21">
-      <c r="A50" s="4">
-        <v>13039</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C50" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="D50" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0.17</v>
-      </c>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
-      <c r="L50" s="4"/>
-      <c r="M50" s="4"/>
-      <c r="N50" s="4"/>
-      <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
-      <c r="Q50" s="4"/>
-      <c r="R50" s="4"/>
-      <c r="S50" s="4"/>
+      <c r="F50" s="13"/>
+      <c r="G50" s="13"/>
+      <c r="H50" s="13"/>
+      <c r="I50" s="13"/>
+      <c r="J50" s="13"/>
+      <c r="K50" s="13"/>
+      <c r="L50" s="13"/>
+      <c r="M50" s="13"/>
+      <c r="N50" s="13"/>
+      <c r="O50" s="13"/>
+      <c r="P50" s="13"/>
+      <c r="Q50" s="13"/>
+      <c r="R50" s="13"/>
+      <c r="S50" s="13"/>
       <c r="T50" s="13"/>
       <c r="U50" s="13"/>
     </row>
-    <row r="51" spans="1:21" s="15" customFormat="1">
-      <c r="A51" s="14">
+    <row r="51" spans="1:21">
+      <c r="A51" s="4">
+        <v>13039</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C51" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E51" s="4">
+        <v>0.17</v>
+      </c>
+      <c r="F51" s="4"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="4"/>
+      <c r="L51" s="4"/>
+      <c r="M51" s="4"/>
+      <c r="N51" s="4"/>
+      <c r="O51" s="4"/>
+      <c r="P51" s="4"/>
+      <c r="Q51" s="4"/>
+      <c r="R51" s="4"/>
+      <c r="S51" s="4"/>
+      <c r="T51" s="13"/>
+      <c r="U51" s="13"/>
+    </row>
+    <row r="52" spans="1:21" s="25" customFormat="1">
+      <c r="A52" s="23">
         <v>13041</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B52" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C52" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="D51" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E51" s="14">
+      <c r="D52" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E52" s="23">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="14"/>
-      <c r="I51" s="14"/>
-      <c r="J51" s="14"/>
-      <c r="K51" s="14"/>
-      <c r="L51" s="14"/>
-      <c r="M51" s="14"/>
-      <c r="N51" s="14"/>
-      <c r="O51" s="14"/>
-      <c r="P51" s="14"/>
-      <c r="Q51" s="14"/>
-      <c r="R51" s="14"/>
-      <c r="S51" s="14"/>
-      <c r="T51" s="14"/>
-      <c r="U51" s="14"/>
-    </row>
-    <row r="52" spans="1:21" s="15" customFormat="1">
-      <c r="A52" s="14">
+      <c r="F52" s="23"/>
+      <c r="G52" s="23"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+      <c r="K52" s="23"/>
+      <c r="L52" s="23"/>
+      <c r="M52" s="23"/>
+      <c r="N52" s="23"/>
+      <c r="O52" s="23"/>
+      <c r="P52" s="23"/>
+      <c r="Q52" s="23"/>
+      <c r="R52" s="23"/>
+      <c r="S52" s="23"/>
+      <c r="T52" s="23"/>
+      <c r="U52" s="23"/>
+    </row>
+    <row r="53" spans="1:21" s="25" customFormat="1">
+      <c r="A53" s="23">
         <v>13046</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B53" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C53" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="D52" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E52" s="14">
+      <c r="D53" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E53" s="23">
         <v>0.22</v>
       </c>
-      <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="14"/>
-      <c r="I52" s="14"/>
-      <c r="J52" s="14"/>
-      <c r="K52" s="14"/>
-      <c r="L52" s="14"/>
-      <c r="M52" s="14"/>
-      <c r="N52" s="14"/>
-      <c r="O52" s="14"/>
-      <c r="P52" s="14"/>
-      <c r="Q52" s="14"/>
-      <c r="R52" s="14"/>
-      <c r="S52" s="14"/>
-      <c r="T52" s="14"/>
-      <c r="U52" s="14"/>
-    </row>
-    <row r="53" spans="1:21">
-      <c r="A53" s="4">
-        <v>13047</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C53" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D53" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E53" s="4">
-        <v>0.11</v>
-      </c>
-      <c r="F53" s="4"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="4"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="4"/>
-      <c r="P53" s="4"/>
-      <c r="Q53" s="4"/>
-      <c r="R53" s="4"/>
-      <c r="S53" s="4"/>
-      <c r="T53" s="13"/>
-      <c r="U53" s="13"/>
+      <c r="F53" s="23"/>
+      <c r="G53" s="23"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
+      <c r="J53" s="23"/>
+      <c r="K53" s="23"/>
+      <c r="L53" s="23"/>
+      <c r="M53" s="23"/>
+      <c r="N53" s="23"/>
+      <c r="O53" s="23"/>
+      <c r="P53" s="23"/>
+      <c r="Q53" s="23"/>
+      <c r="R53" s="23"/>
+      <c r="S53" s="23"/>
+      <c r="T53" s="23"/>
+      <c r="U53" s="23"/>
     </row>
     <row r="54" spans="1:21">
       <c r="A54" s="4">
-        <v>13052</v>
+        <v>13047</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D54" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E54" s="4">
-        <v>0.22</v>
+        <v>0.11</v>
       </c>
       <c r="F54" s="4"/>
       <c r="G54" s="4"/>
@@ -3191,19 +3199,19 @@
     </row>
     <row r="55" spans="1:21">
       <c r="A55" s="4">
-        <v>13053</v>
+        <v>13052</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D55" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E55" s="4">
-        <v>0.16</v>
+        <v>0.22</v>
       </c>
       <c r="F55" s="4"/>
       <c r="G55" s="4"/>
@@ -3224,19 +3232,19 @@
     </row>
     <row r="56" spans="1:21">
       <c r="A56" s="4">
-        <v>13061</v>
+        <v>13053</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D56" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E56" s="4">
-        <v>0.22</v>
+        <v>0.16</v>
       </c>
       <c r="F56" s="4"/>
       <c r="G56" s="4"/>
@@ -3255,120 +3263,120 @@
       <c r="T56" s="13"/>
       <c r="U56" s="13"/>
     </row>
-    <row r="57" spans="1:21" s="15" customFormat="1">
-      <c r="A57" s="14">
+    <row r="57" spans="1:21">
+      <c r="A57" s="4">
+        <v>13061</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C57" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E57" s="4">
+        <v>0.22</v>
+      </c>
+      <c r="F57" s="4"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="4"/>
+      <c r="L57" s="4"/>
+      <c r="M57" s="4"/>
+      <c r="N57" s="4"/>
+      <c r="O57" s="4"/>
+      <c r="P57" s="4"/>
+      <c r="Q57" s="4"/>
+      <c r="R57" s="4"/>
+      <c r="S57" s="4"/>
+      <c r="T57" s="13"/>
+      <c r="U57" s="13"/>
+    </row>
+    <row r="58" spans="1:21" s="25" customFormat="1">
+      <c r="A58" s="23">
         <v>13064</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B58" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="C57" s="12" t="s">
+      <c r="C58" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D58" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E58" s="23">
+        <v>0.22</v>
+      </c>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="23"/>
+      <c r="I58" s="23"/>
+      <c r="J58" s="23"/>
+      <c r="K58" s="23"/>
+      <c r="L58" s="23"/>
+      <c r="M58" s="23"/>
+      <c r="N58" s="23"/>
+      <c r="O58" s="23"/>
+      <c r="P58" s="23"/>
+      <c r="Q58" s="23"/>
+      <c r="R58" s="23"/>
+      <c r="S58" s="23"/>
+      <c r="T58" s="23"/>
+      <c r="U58" s="23"/>
+    </row>
+    <row r="59" spans="1:21" s="15" customFormat="1">
+      <c r="A59" s="14">
+        <v>13069</v>
+      </c>
+      <c r="B59" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C59" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="D59" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E57" s="14">
-        <v>0.22</v>
-      </c>
-      <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="14"/>
-      <c r="I57" s="14"/>
-      <c r="J57" s="14"/>
-      <c r="K57" s="14"/>
-      <c r="L57" s="14"/>
-      <c r="M57" s="14"/>
-      <c r="N57" s="14"/>
-      <c r="O57" s="14"/>
-      <c r="P57" s="14"/>
-      <c r="Q57" s="14"/>
-      <c r="R57" s="14"/>
-      <c r="S57" s="14"/>
-      <c r="T57" s="14"/>
-      <c r="U57" s="14"/>
-    </row>
-    <row r="58" spans="1:21">
-      <c r="A58" s="4">
-        <v>13069</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C58" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D58" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E58" s="4">
+      <c r="E59" s="14">
         <v>0.11</v>
       </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
-      <c r="J58" s="4"/>
-      <c r="K58" s="4"/>
-      <c r="L58" s="4"/>
-      <c r="M58" s="4"/>
-      <c r="N58" s="4"/>
-      <c r="O58" s="4"/>
-      <c r="P58" s="4"/>
-      <c r="Q58" s="4"/>
-      <c r="R58" s="4"/>
-      <c r="S58" s="4"/>
-      <c r="T58" s="13"/>
-      <c r="U58" s="13"/>
-    </row>
-    <row r="59" spans="1:21">
-      <c r="A59" s="4">
-        <v>13070</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C59" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="E59" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4"/>
-      <c r="K59" s="4"/>
-      <c r="L59" s="4"/>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4"/>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4"/>
-      <c r="Q59" s="4"/>
-      <c r="R59" s="4"/>
-      <c r="S59" s="4"/>
-      <c r="T59" s="13"/>
-      <c r="U59" s="13"/>
+      <c r="F59" s="14"/>
+      <c r="G59" s="14"/>
+      <c r="H59" s="14"/>
+      <c r="I59" s="14"/>
+      <c r="J59" s="14"/>
+      <c r="K59" s="14"/>
+      <c r="L59" s="14"/>
+      <c r="M59" s="14"/>
+      <c r="N59" s="14"/>
+      <c r="O59" s="14"/>
+      <c r="P59" s="14"/>
+      <c r="Q59" s="14"/>
+      <c r="R59" s="14"/>
+      <c r="S59" s="14"/>
+      <c r="T59" s="14"/>
+      <c r="U59" s="14"/>
     </row>
     <row r="60" spans="1:21">
       <c r="A60" s="4">
-        <v>14106</v>
+        <v>13070</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>65</v>
+        <v>22</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="D60" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E60" s="4">
-        <v>0.22</v>
+        <v>0.06</v>
       </c>
       <c r="F60" s="4"/>
       <c r="G60" s="4"/>
@@ -3389,19 +3397,19 @@
     </row>
     <row r="61" spans="1:21">
       <c r="A61" s="4">
-        <v>14107</v>
+        <v>14106</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C61" s="10" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
       <c r="D61" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E61" s="4">
-        <v>0.45</v>
+        <v>0.22</v>
       </c>
       <c r="F61" s="4"/>
       <c r="G61" s="4"/>
@@ -3422,19 +3430,19 @@
     </row>
     <row r="62" spans="1:21">
       <c r="A62" s="4">
-        <v>14109</v>
+        <v>14107</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E62" s="4">
-        <v>0.17</v>
+        <v>0.45</v>
       </c>
       <c r="F62" s="4"/>
       <c r="G62" s="4"/>
@@ -3455,19 +3463,19 @@
     </row>
     <row r="63" spans="1:21">
       <c r="A63" s="4">
-        <v>14110</v>
+        <v>14109</v>
       </c>
       <c r="B63" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D63" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E63" s="4">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
       <c r="F63" s="4"/>
       <c r="G63" s="4"/>
@@ -3488,19 +3496,19 @@
     </row>
     <row r="64" spans="1:21">
       <c r="A64" s="4">
-        <v>14112</v>
+        <v>14110</v>
       </c>
       <c r="B64" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="D64" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E64" s="4">
-        <v>0.34</v>
+        <v>0.11</v>
       </c>
       <c r="F64" s="4"/>
       <c r="G64" s="4"/>
@@ -3521,19 +3529,19 @@
     </row>
     <row r="65" spans="1:21">
       <c r="A65" s="4">
-        <v>14115</v>
+        <v>14112</v>
       </c>
       <c r="B65" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="D65" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E65" s="4">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="F65" s="4"/>
       <c r="G65" s="4"/>
@@ -3554,19 +3562,19 @@
     </row>
     <row r="66" spans="1:21">
       <c r="A66" s="4">
-        <v>14117</v>
+        <v>14115</v>
       </c>
       <c r="B66" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="D66" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E66" s="4">
-        <v>0.39</v>
+        <v>0.22</v>
       </c>
       <c r="F66" s="4"/>
       <c r="G66" s="4"/>
@@ -3587,19 +3595,19 @@
     </row>
     <row r="67" spans="1:21">
       <c r="A67" s="4">
-        <v>14124</v>
+        <v>14117</v>
       </c>
       <c r="B67" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>41</v>
+        <v>52</v>
       </c>
       <c r="D67" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E67" s="4">
-        <v>0.78</v>
+        <v>0.39</v>
       </c>
       <c r="F67" s="4"/>
       <c r="G67" s="4"/>
@@ -3620,19 +3628,19 @@
     </row>
     <row r="68" spans="1:21">
       <c r="A68" s="4">
-        <v>14126</v>
+        <v>14124</v>
       </c>
       <c r="B68" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D68" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E68" s="4">
-        <v>0.17</v>
+        <v>0.78</v>
       </c>
       <c r="F68" s="4"/>
       <c r="G68" s="4"/>
@@ -3653,19 +3661,19 @@
     </row>
     <row r="69" spans="1:21">
       <c r="A69" s="4">
-        <v>14135</v>
+        <v>14126</v>
       </c>
       <c r="B69" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="D69" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E69" s="4">
-        <v>0.22</v>
+        <v>0.17</v>
       </c>
       <c r="F69" s="4"/>
       <c r="G69" s="4"/>
@@ -3686,19 +3694,19 @@
     </row>
     <row r="70" spans="1:21">
       <c r="A70" s="4">
-        <v>14136</v>
+        <v>14135</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C70" s="10" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="D70" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E70" s="4">
-        <v>0.11</v>
+        <v>0.22</v>
       </c>
       <c r="F70" s="4"/>
       <c r="G70" s="4"/>
@@ -3719,19 +3727,19 @@
     </row>
     <row r="71" spans="1:21">
       <c r="A71" s="4">
-        <v>14137</v>
+        <v>14136</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C71" s="10" t="s">
-        <v>44</v>
+        <v>66</v>
       </c>
       <c r="D71" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E71" s="4">
-        <v>0.17</v>
+        <v>0.11</v>
       </c>
       <c r="F71" s="4"/>
       <c r="G71" s="4"/>
@@ -3752,13 +3760,13 @@
     </row>
     <row r="72" spans="1:21">
       <c r="A72" s="4">
-        <v>14138</v>
+        <v>14137</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C72" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D72" s="10" t="s">
         <v>68</v>
@@ -3785,13 +3793,13 @@
     </row>
     <row r="73" spans="1:21">
       <c r="A73" s="4">
-        <v>14144</v>
+        <v>14138</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
       <c r="D73" s="10" t="s">
         <v>68</v>
@@ -3818,19 +3826,19 @@
     </row>
     <row r="74" spans="1:21">
       <c r="A74" s="4">
-        <v>14147</v>
+        <v>14144</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="D74" s="10" t="s">
         <v>68</v>
       </c>
       <c r="E74" s="4">
-        <v>0.45</v>
+        <v>0.17</v>
       </c>
       <c r="F74" s="4"/>
       <c r="G74" s="4"/>
@@ -3849,67 +3857,104 @@
       <c r="T74" s="13"/>
       <c r="U74" s="13"/>
     </row>
-    <row r="75" spans="1:21" s="15" customFormat="1">
-      <c r="A75" s="14">
+    <row r="75" spans="1:21">
+      <c r="A75" s="4">
+        <v>14147</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="E75" s="4">
+        <v>0.45</v>
+      </c>
+      <c r="F75" s="4"/>
+      <c r="G75" s="4"/>
+      <c r="H75" s="4"/>
+      <c r="I75" s="4"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="4"/>
+      <c r="L75" s="4"/>
+      <c r="M75" s="4"/>
+      <c r="N75" s="4"/>
+      <c r="O75" s="4"/>
+      <c r="P75" s="4"/>
+      <c r="Q75" s="4"/>
+      <c r="R75" s="4"/>
+      <c r="S75" s="4"/>
+      <c r="T75" s="13"/>
+      <c r="U75" s="13"/>
+    </row>
+    <row r="76" spans="1:21" s="25" customFormat="1">
+      <c r="A76" s="23">
         <v>14772</v>
       </c>
-      <c r="B75" s="14"/>
-      <c r="C75" s="12"/>
-      <c r="D75" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E75" s="14">
+      <c r="B76" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" s="26"/>
+      <c r="D76" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E76" s="23">
         <v>0.28000000000000003</v>
       </c>
-      <c r="F75" s="14"/>
-      <c r="G75" s="14"/>
-      <c r="H75" s="14"/>
-      <c r="I75" s="14"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14"/>
-      <c r="M75" s="14"/>
-      <c r="N75" s="14"/>
-      <c r="O75" s="14"/>
-      <c r="P75" s="14"/>
-      <c r="Q75" s="14"/>
-      <c r="R75" s="14"/>
-      <c r="S75" s="14"/>
-      <c r="T75" s="14"/>
-      <c r="U75" s="14"/>
-    </row>
-    <row r="76" spans="1:21" s="15" customFormat="1">
-      <c r="A76" s="14">
+      <c r="F76" s="23"/>
+      <c r="G76" s="23"/>
+      <c r="H76" s="23"/>
+      <c r="I76" s="23"/>
+      <c r="J76" s="23"/>
+      <c r="K76" s="23"/>
+      <c r="L76" s="23"/>
+      <c r="M76" s="23"/>
+      <c r="N76" s="23"/>
+      <c r="O76" s="23"/>
+      <c r="P76" s="23"/>
+      <c r="Q76" s="23"/>
+      <c r="R76" s="23"/>
+      <c r="S76" s="23"/>
+      <c r="T76" s="23"/>
+      <c r="U76" s="23"/>
+    </row>
+    <row r="77" spans="1:21" s="25" customFormat="1">
+      <c r="A77" s="23">
         <v>14775</v>
       </c>
-      <c r="B76" s="14"/>
-      <c r="C76" s="12"/>
-      <c r="D76" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="E76" s="14">
+      <c r="B77" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C77" s="26"/>
+      <c r="D77" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="E77" s="23">
         <v>0.34</v>
       </c>
-      <c r="F76" s="14"/>
-      <c r="G76" s="14"/>
-      <c r="H76" s="14"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
-      <c r="K76" s="14"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="14"/>
-      <c r="N76" s="14"/>
-      <c r="O76" s="14"/>
-      <c r="P76" s="14"/>
-      <c r="Q76" s="14"/>
-      <c r="R76" s="14"/>
-      <c r="S76" s="14"/>
-      <c r="T76" s="14"/>
-      <c r="U76" s="14"/>
+      <c r="F77" s="23"/>
+      <c r="G77" s="23"/>
+      <c r="H77" s="23"/>
+      <c r="I77" s="23"/>
+      <c r="J77" s="23"/>
+      <c r="K77" s="23"/>
+      <c r="L77" s="23"/>
+      <c r="M77" s="23"/>
+      <c r="N77" s="23"/>
+      <c r="O77" s="23"/>
+      <c r="P77" s="23"/>
+      <c r="Q77" s="23"/>
+      <c r="R77" s="23"/>
+      <c r="S77" s="23"/>
+      <c r="T77" s="23"/>
+      <c r="U77" s="23"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U76">
-    <sortCondition ref="A40"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U77">
+    <sortCondition ref="A41"/>
   </sortState>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>